<commit_message>
Enemy collision and global enums
Updated collision shapes for new 48x48 sprites.
Updated global enums and references for enemy resources.
</commit_message>
<xml_diff>
--- a/sprite_sheet.xlsx
+++ b/sprite_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nthnl\Desktop\Code\Flashtrek-2.0-Godot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2B9447-0A00-4A0B-B558-2FAFDACE750F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E6ADDF-4446-4DD9-B4CE-A5C651DD1005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9480D77A-E5C1-4096-97D1-11AE8DADC1A6}"/>
   </bookViews>
@@ -272,9 +272,6 @@
     <t>Nebula-Class (Phoenix variant)</t>
   </si>
   <si>
-    <t>Hysperian Monaveen</t>
-  </si>
-  <si>
     <t>Risian Luxury Cruiser</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Jem'Hadar</t>
+  </si>
+  <si>
+    <t>Monaveen</t>
   </si>
 </sst>
 </file>
@@ -398,6 +398,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>40822</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>162463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D03B2DE-2F4E-75A3-B7D4-C105E6187848}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="653143" y="2598964"/>
+          <a:ext cx="14505214" cy="7142928"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A46386-5A4D-4B73-8EAB-C9B2C9DD0814}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.4"/>
@@ -790,13 +856,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -843,7 +909,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -890,7 +956,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -928,7 +994,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>41</v>
@@ -979,7 +1045,7 @@
         <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
         <v>55</v>
@@ -1065,40 +1131,40 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
         <v>78</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>79</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>80</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>81</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>82</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>83</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>84</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>85</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>86</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>87</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>88</v>
-      </c>
-      <c r="O8" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1108,5 +1174,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP Ship data refactor, tool scripts, addon changes
Various strict typing additions to many scripts.
Ship data/stats refactor using Resources and JSON data (in progress)
Tool script for creating GalaxyMap resources (for neighbor maps and warping)
Tool script for generating PackedVector2Array collision shape from sprite sheet
Tool script for creating ship resources (stats and data) (depricatedby JSON loading)

Changed warp video to tunnel effect shader
Removed Sprite Painter addon
</commit_message>
<xml_diff>
--- a/sprite_sheet.xlsx
+++ b/sprite_sheet.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nthnl\Desktop\Code\Flashtrek-2.0-Godot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nthnl\Desktop\Code\Flashtrek-2.0-Godot-4.4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E6ADDF-4446-4DD9-B4CE-A5C651DD1005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7BD51F-D537-41F3-9295-CB2F8E6F3170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9480D77A-E5C1-4096-97D1-11AE8DADC1A6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprites" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,9 +92,6 @@
     <t>daSpu'-Class</t>
   </si>
   <si>
-    <t>Klingon Bird-of-Prey (Discovery era)</t>
-  </si>
-  <si>
     <t>Walker-Class</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Monaveen</t>
+  </si>
+  <si>
+    <t>Klingon_Bird_of_Prey</t>
   </si>
 </sst>
 </file>
@@ -379,10 +379,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,13 +405,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>40822</xdr:colOff>
+      <xdr:colOff>40821</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>204107</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>54428</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>162463</xdr:rowOff>
     </xdr:to>
@@ -443,8 +443,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="653143" y="2598964"/>
-          <a:ext cx="14505214" cy="7142928"/>
+          <a:off x="653142" y="2598964"/>
+          <a:ext cx="26806072" cy="7142928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -785,65 +785,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A46386-5A4D-4B73-8EAB-C9B2C9DD0814}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="3" width="28.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="15" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="15" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="3">
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>48</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>96</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>144</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>192</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>240</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>288</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>336</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>384</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>432</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>480</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>528</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="2">
         <v>576</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="2">
         <v>624</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -856,13 +853,13 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -890,7 +887,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>48</v>
       </c>
       <c r="B3" t="s">
@@ -906,265 +903,265 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>25</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>96</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>34</v>
-      </c>
-      <c r="K4" t="s">
-        <v>35</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
       </c>
       <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
-      </c>
-      <c r="O4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>144</v>
       </c>
       <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>43</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>44</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>46</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>47</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>48</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>49</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>50</v>
-      </c>
-      <c r="O5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>192</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>58</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>59</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>60</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>61</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>62</v>
-      </c>
-      <c r="O6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>240</v>
       </c>
       <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" t="s">
         <v>65</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>68</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>69</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>70</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>71</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>72</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>73</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>74</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>75</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>76</v>
-      </c>
-      <c r="O7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>288</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="3"/>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
         <v>78</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>79</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>80</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>81</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>82</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>83</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>84</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>85</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>86</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>87</v>
-      </c>
-      <c r="O8" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>